<commit_message>
Add SKRPABE010 C115360 to BOM and update counts
- Alps SKRPABE010: C115360確定（JLCPCB在庫54355個確認済み）
- キースイッチ数: 60→68個（66キー+ショルダー2個）
- ダイオード数: Claude.md内を62→66個に修正

Co-Authored-By: Claude Sonnet 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/bom/cyberdeck_bom.xlsx
+++ b/bom/cyberdeck_bom.xlsx
@@ -601,7 +601,7 @@
     <col width="28" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="8" customWidth="1" min="6" max="6"/>
-    <col width="48" customWidth="1" min="7" max="7"/>
+    <col width="52" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="22" customHeight="1">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="E19" s="12" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>C115360</t>
         </is>
       </c>
       <c r="F19" s="12" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="G19" s="13" t="inlineStr">
         <is>
-          <t>66キー + ショルダー2個 / 4.2×3.2mm SMD</t>
+          <t>66キー + ショルダー2個 / 4.2×3.2mm SMD / JLCPCB在庫54355個確認済み</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Change analog stick to 3DS slide pad, add FPC connector
- アナログスティック: PSP互換品 → 3DSスライドパッド（感触優先）
- FPCコネクタ追加: AFC01-S06FCA-00 (C262655) / 6P 0.5mm Bottom Contact ZIF
- BOM・Claude.md・PROJECT_PLAN.md 全更新
- 秋月JT8P: キャップ非互換のため不採用

Co-Authored-By: Claude Sonnet 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/bom/cyberdeck_bom.xlsx
+++ b/bom/cyberdeck_bom.xlsx
@@ -10,7 +10,7 @@
     <sheet name="BOM" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'BOM'!$A$1:$G$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'BOM'!$A$1:$G$38</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -586,7 +586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C21" s="14" t="inlineStr">
         <is>
-          <t>PSP互換アナログスティック</t>
+          <t>3DSスライドパッド</t>
         </is>
       </c>
       <c r="D21" s="14" t="inlineStr">
@@ -1377,44 +1377,44 @@
       </c>
       <c r="G21" s="15" t="inlineStr">
         <is>
-          <t>カーソル操作用 / 別途購入（AliExpress）</t>
+          <t>カーソル操作用 / FPC 6ピン 0.5mmピッチ 0.3mm厚 / 別途購入（AliExpress or 中古）</t>
         </is>
       </c>
     </row>
     <row r="22" ht="18" customHeight="1">
-      <c r="A22" s="16" t="inlineStr">
-        <is>
-          <t>オーディオ</t>
-        </is>
-      </c>
-      <c r="B22" s="16" t="inlineStr">
-        <is>
-          <t>I2Sアンプ</t>
-        </is>
-      </c>
-      <c r="C22" s="16" t="inlineStr">
-        <is>
-          <t>MAX98357AEWL+T</t>
-        </is>
-      </c>
-      <c r="D22" s="16" t="inlineStr">
-        <is>
-          <t>MAX98357AEWL+T</t>
-        </is>
-      </c>
-      <c r="E22" s="16" t="inlineStr">
-        <is>
-          <t>C2682619</t>
-        </is>
-      </c>
-      <c r="F22" s="16" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G22" s="17" t="inlineStr">
-        <is>
-          <t>ステレオ構成 / I2S入力</t>
+      <c r="A22" s="14" t="inlineStr">
+        <is>
+          <t>入力</t>
+        </is>
+      </c>
+      <c r="B22" s="14" t="inlineStr">
+        <is>
+          <t>FPCコネクタ（スティック用）</t>
+        </is>
+      </c>
+      <c r="C22" s="14" t="inlineStr">
+        <is>
+          <t>AFC01-S06FCA-00</t>
+        </is>
+      </c>
+      <c r="D22" s="14" t="inlineStr">
+        <is>
+          <t>AFC01-S06FCA-00</t>
+        </is>
+      </c>
+      <c r="E22" s="14" t="inlineStr">
+        <is>
+          <t>C262655</t>
+        </is>
+      </c>
+      <c r="F22" s="14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G22" s="15" t="inlineStr">
+        <is>
+          <t>6P 0.5mmピッチ Bottom Contact ZIF / 3DSスライドパッド接続用 / JLCPCB在庫52426個確認済み</t>
         </is>
       </c>
     </row>
@@ -1426,32 +1426,32 @@
       </c>
       <c r="B23" s="16" t="inlineStr">
         <is>
-          <t>スピーカー</t>
+          <t>I2Sアンプ</t>
         </is>
       </c>
       <c r="C23" s="16" t="inlineStr">
         <is>
-          <t>マイクロスピーカー 8Ω</t>
+          <t>MAX98357AEWL+T</t>
         </is>
       </c>
       <c r="D23" s="16" t="inlineStr">
         <is>
-          <t>秋月P-12494 or P-12495</t>
+          <t>MAX98357AEWL+T</t>
         </is>
       </c>
       <c r="E23" s="16" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>C2682619</t>
         </is>
       </c>
       <c r="F23" s="16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G23" s="17" t="inlineStr">
         <is>
-          <t>23×16×4.6mm / 片チャンネルのみ / 別途購入（秋月）</t>
+          <t>ステレオ構成 / I2S入力</t>
         </is>
       </c>
     </row>
@@ -1463,106 +1463,106 @@
       </c>
       <c r="B24" s="16" t="inlineStr">
         <is>
+          <t>スピーカー</t>
+        </is>
+      </c>
+      <c r="C24" s="16" t="inlineStr">
+        <is>
+          <t>マイクロスピーカー 8Ω</t>
+        </is>
+      </c>
+      <c r="D24" s="16" t="inlineStr">
+        <is>
+          <t>秋月P-12494 or P-12495</t>
+        </is>
+      </c>
+      <c r="E24" s="16" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F24" s="16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G24" s="17" t="inlineStr">
+        <is>
+          <t>23×16×4.6mm / 片チャンネルのみ / 別途購入（秋月）</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="18" customHeight="1">
+      <c r="A25" s="16" t="inlineStr">
+        <is>
+          <t>オーディオ</t>
+        </is>
+      </c>
+      <c r="B25" s="16" t="inlineStr">
+        <is>
           <t>イヤホンジャック</t>
         </is>
       </c>
-      <c r="C24" s="16" t="inlineStr">
+      <c r="C25" s="16" t="inlineStr">
         <is>
           <t>3.5mm TRRS SMT</t>
         </is>
       </c>
-      <c r="D24" s="16" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="E24" s="16" t="inlineStr">
+      <c r="D25" s="16" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="E25" s="16" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="F24" s="16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G24" s="17" t="inlineStr">
+      <c r="F25" s="16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G25" s="17" t="inlineStr">
         <is>
           <t>挿入時スピーカーミュート / 型番未定</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="18" customHeight="1">
-      <c r="A25" s="18" t="inlineStr">
+    <row r="26" ht="18" customHeight="1">
+      <c r="A26" s="18" t="inlineStr">
         <is>
           <t>汎用</t>
         </is>
       </c>
-      <c r="B25" s="18" t="inlineStr">
+      <c r="B26" s="18" t="inlineStr">
         <is>
           <t>NchMOSFET</t>
         </is>
       </c>
-      <c r="C25" s="18" t="inlineStr">
+      <c r="C26" s="18" t="inlineStr">
         <is>
           <t>BSS138</t>
         </is>
       </c>
-      <c r="D25" s="18" t="inlineStr">
+      <c r="D26" s="18" t="inlineStr">
         <is>
           <t>BSS138</t>
         </is>
       </c>
-      <c r="E25" s="18" t="inlineStr">
+      <c r="E26" s="18" t="inlineStr">
         <is>
           <t>C52895</t>
         </is>
       </c>
-      <c r="F25" s="18" t="inlineStr">
+      <c r="F26" s="18" t="inlineStr">
         <is>
           <t>適宜</t>
         </is>
       </c>
-      <c r="G25" s="19" t="inlineStr">
+      <c r="G26" s="19" t="inlineStr">
         <is>
           <t>レベルシフト等</t>
-        </is>
-      </c>
-    </row>
-    <row r="26" ht="18" customHeight="1">
-      <c r="A26" s="20" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="B26" s="20" t="inlineStr">
-        <is>
-          <t>電源LED（緑）</t>
-        </is>
-      </c>
-      <c r="C26" s="20" t="inlineStr">
-        <is>
-          <t>緑色LED</t>
-        </is>
-      </c>
-      <c r="D26" s="20" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="E26" s="20" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="F26" s="20" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G26" s="21" t="inlineStr">
-        <is>
-          <t>TPS61023出力（5V）から電流制限抵抗で駆動</t>
         </is>
       </c>
     </row>
@@ -1574,12 +1574,12 @@
       </c>
       <c r="B27" s="20" t="inlineStr">
         <is>
-          <t>充電中LED（橙）</t>
+          <t>電源LED（緑）</t>
         </is>
       </c>
       <c r="C27" s="20" t="inlineStr">
         <is>
-          <t>橙色LED</t>
+          <t>緑色LED</t>
         </is>
       </c>
       <c r="D27" s="20" t="inlineStr">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="G27" s="21" t="inlineStr">
         <is>
-          <t>RP2040 GP24 / BQ25895 I2C読み</t>
+          <t>TPS61023出力（5V）から電流制限抵抗で駆動</t>
         </is>
       </c>
     </row>
@@ -1611,12 +1611,12 @@
       </c>
       <c r="B28" s="20" t="inlineStr">
         <is>
-          <t>充電完了LED（緑）</t>
+          <t>充電中LED（橙）</t>
         </is>
       </c>
       <c r="C28" s="20" t="inlineStr">
         <is>
-          <t>緑色LED</t>
+          <t>橙色LED</t>
         </is>
       </c>
       <c r="D28" s="20" t="inlineStr">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="G28" s="21" t="inlineStr">
         <is>
-          <t>RP2040 GP25 / BQ25895 I2C読み</t>
+          <t>RP2040 GP24 / BQ25895 I2C読み</t>
         </is>
       </c>
     </row>
@@ -1648,69 +1648,69 @@
       </c>
       <c r="B29" s="20" t="inlineStr">
         <is>
+          <t>充電完了LED（緑）</t>
+        </is>
+      </c>
+      <c r="C29" s="20" t="inlineStr">
+        <is>
+          <t>緑色LED</t>
+        </is>
+      </c>
+      <c r="D29" s="20" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="E29" s="20" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="F29" s="20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G29" s="21" t="inlineStr">
+        <is>
+          <t>RP2040 GP25 / BQ25895 I2C読み</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="18" customHeight="1">
+      <c r="A30" s="20" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="B30" s="20" t="inlineStr">
+        <is>
           <t>ACT LED</t>
         </is>
       </c>
-      <c r="C29" s="20" t="inlineStr">
+      <c r="C30" s="20" t="inlineStr">
         <is>
           <t>緑色LED</t>
         </is>
       </c>
-      <c r="D29" s="20" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="E29" s="20" t="inlineStr">
+      <c r="D30" s="20" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="E30" s="20" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="F29" s="20" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G29" s="21" t="inlineStr">
+      <c r="F30" s="20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G30" s="21" t="inlineStr">
         <is>
           <t>RP2040 GP26（ADC0兼用）/ SBC経由制御</t>
-        </is>
-      </c>
-    </row>
-    <row r="30" ht="18" customHeight="1">
-      <c r="A30" s="22" t="inlineStr">
-        <is>
-          <t>冷却</t>
-        </is>
-      </c>
-      <c r="B30" s="22" t="inlineStr">
-        <is>
-          <t>フラットヒートパイプ</t>
-        </is>
-      </c>
-      <c r="C30" s="22" t="inlineStr">
-        <is>
-          <t>3mm厚フラット銅製ヒートパイプ</t>
-        </is>
-      </c>
-      <c r="D30" s="22" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="E30" s="22" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F30" s="22" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G30" s="23" t="inlineStr">
-        <is>
-          <t>SoC→90度曲げ→バッテリー上端 / 別途購入</t>
         </is>
       </c>
     </row>
@@ -1722,69 +1722,69 @@
       </c>
       <c r="B31" s="22" t="inlineStr">
         <is>
+          <t>フラットヒートパイプ</t>
+        </is>
+      </c>
+      <c r="C31" s="22" t="inlineStr">
+        <is>
+          <t>3mm厚フラット銅製ヒートパイプ</t>
+        </is>
+      </c>
+      <c r="D31" s="22" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="E31" s="22" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F31" s="22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G31" s="23" t="inlineStr">
+        <is>
+          <t>SoC→90度曲げ→バッテリー上端 / 別途購入</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" ht="18" customHeight="1">
+      <c r="A32" s="22" t="inlineStr">
+        <is>
+          <t>冷却</t>
+        </is>
+      </c>
+      <c r="B32" s="22" t="inlineStr">
+        <is>
           <t>ヒートシンク</t>
         </is>
       </c>
-      <c r="C31" s="22" t="inlineStr">
+      <c r="C32" s="22" t="inlineStr">
         <is>
           <t>小型ヒートシンク</t>
         </is>
       </c>
-      <c r="D31" s="22" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="E31" s="22" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F31" s="22" t="inlineStr">
+      <c r="D32" s="22" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="E32" s="22" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F32" s="22" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="G31" s="23" t="inlineStr">
+      <c r="G32" s="23" t="inlineStr">
         <is>
           <t>14×9×4mm程度 / サーマルパッド必要 / 別途購入</t>
-        </is>
-      </c>
-    </row>
-    <row r="32" ht="18" customHeight="1">
-      <c r="A32" s="24" t="inlineStr">
-        <is>
-          <t>コネクタ</t>
-        </is>
-      </c>
-      <c r="B32" s="24" t="inlineStr">
-        <is>
-          <t>外部USB-Cレセプタクル</t>
-        </is>
-      </c>
-      <c r="C32" s="24" t="inlineStr">
-        <is>
-          <t>USB-C レセプタクル SMT</t>
-        </is>
-      </c>
-      <c r="D32" s="24" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="E32" s="24" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="F32" s="24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G32" s="25" t="inlineStr">
-        <is>
-          <t>DATAポート（VL812 downstream 1）</t>
         </is>
       </c>
     </row>
@@ -1796,12 +1796,12 @@
       </c>
       <c r="B33" s="24" t="inlineStr">
         <is>
-          <t>外部USB-Aレセプタクル</t>
+          <t>外部USB-Cレセプタクル</t>
         </is>
       </c>
       <c r="C33" s="24" t="inlineStr">
         <is>
-          <t>USB-A レセプタクル SMT</t>
+          <t>USB-C レセプタクル SMT</t>
         </is>
       </c>
       <c r="D33" s="24" t="inlineStr">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="G33" s="25" t="inlineStr">
         <is>
-          <t>汎用USBポート（VL812 downstream 2）</t>
+          <t>DATAポート（VL812 downstream 1）</t>
         </is>
       </c>
     </row>
@@ -1833,12 +1833,12 @@
       </c>
       <c r="B34" s="24" t="inlineStr">
         <is>
-          <t>FPCコネクタ</t>
+          <t>外部USB-Aレセプタクル</t>
         </is>
       </c>
       <c r="C34" s="24" t="inlineStr">
         <is>
-          <t>30ピン 0.5mmピッチ FPCコネクタ</t>
+          <t>USB-A レセプタクル SMT</t>
         </is>
       </c>
       <c r="D34" s="24" t="inlineStr">
@@ -1853,12 +1853,12 @@
       </c>
       <c r="F34" s="24" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G34" s="25" t="inlineStr">
         <is>
-          <t>SBC接続用サブ基板 / ケーブル長は筐体CAD後に確定</t>
+          <t>汎用USBポート（VL812 downstream 2）</t>
         </is>
       </c>
     </row>
@@ -1870,111 +1870,148 @@
       </c>
       <c r="B35" s="24" t="inlineStr">
         <is>
+          <t>FPCコネクタ</t>
+        </is>
+      </c>
+      <c r="C35" s="24" t="inlineStr">
+        <is>
+          <t>30ピン 0.5mmピッチ FPCコネクタ</t>
+        </is>
+      </c>
+      <c r="D35" s="24" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="E35" s="24" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="F35" s="24" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G35" s="25" t="inlineStr">
+        <is>
+          <t>SBC接続用サブ基板 / ケーブル長は筐体CAD後に確定</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="18" customHeight="1">
+      <c r="A36" s="24" t="inlineStr">
+        <is>
+          <t>コネクタ</t>
+        </is>
+      </c>
+      <c r="B36" s="24" t="inlineStr">
+        <is>
           <t>SWDデバッグコネクタ</t>
         </is>
       </c>
-      <c r="C35" s="24" t="inlineStr">
+      <c r="C36" s="24" t="inlineStr">
         <is>
           <t>SWDコネクタ</t>
         </is>
       </c>
-      <c r="D35" s="24" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="E35" s="24" t="inlineStr">
+      <c r="D36" s="24" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="E36" s="24" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="F35" s="24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G35" s="25" t="inlineStr">
+      <c r="F36" s="24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G36" s="25" t="inlineStr">
         <is>
           <t>RP2040デバッグ用</t>
-        </is>
-      </c>
-    </row>
-    <row r="36" ht="18" customHeight="1">
-      <c r="A36" s="26" t="inlineStr">
-        <is>
-          <t>コンデンサ</t>
-        </is>
-      </c>
-      <c r="B36" s="26" t="inlineStr">
-        <is>
-          <t>電解/セラミック 各種</t>
-        </is>
-      </c>
-      <c r="C36" s="26" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="D36" s="26" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="E36" s="26" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F36" s="26" t="inlineStr">
-        <is>
-          <t>多数</t>
-        </is>
-      </c>
-      <c r="G36" s="27" t="inlineStr">
-        <is>
-          <t>回路設計に従い適宜</t>
         </is>
       </c>
     </row>
     <row r="37" ht="18" customHeight="1">
       <c r="A37" s="26" t="inlineStr">
         <is>
+          <t>コンデンサ</t>
+        </is>
+      </c>
+      <c r="B37" s="26" t="inlineStr">
+        <is>
+          <t>電解/セラミック 各種</t>
+        </is>
+      </c>
+      <c r="C37" s="26" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="D37" s="26" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="E37" s="26" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F37" s="26" t="inlineStr">
+        <is>
+          <t>多数</t>
+        </is>
+      </c>
+      <c r="G37" s="27" t="inlineStr">
+        <is>
+          <t>回路設計に従い適宜</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" ht="18" customHeight="1">
+      <c r="A38" s="26" t="inlineStr">
+        <is>
           <t>抵抗</t>
         </is>
       </c>
-      <c r="B37" s="26" t="inlineStr">
+      <c r="B38" s="26" t="inlineStr">
         <is>
           <t>チップ抵抗 各種</t>
         </is>
       </c>
-      <c r="C37" s="26" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="D37" s="26" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="E37" s="26" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="F37" s="26" t="inlineStr">
+      <c r="C38" s="26" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="D38" s="26" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="E38" s="26" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="F38" s="26" t="inlineStr">
         <is>
           <t>多数</t>
         </is>
       </c>
-      <c r="G37" s="27" t="inlineStr">
+      <c r="G38" s="27" t="inlineStr">
         <is>
           <t>回路設計に従い適宜</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G37"/>
+  <autoFilter ref="A1:G38"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix 3DS slide pad FPC connector: 6P/0.5mm -> 4P/1.0mm
- FPCコネクタ修正: C262655(AFC01 6P/0.5mm) → C3170007(Molex 5034800440 4P/1.0mm)
- 3DSスライドパッドは4ピン1.0mmピッチが正しい仕様
- ピンアサイン確定: GND / X軸 / VCC / Y軸
- VCC: 3.3V直結OK（内部ポテンショメータのため電圧スケールのみ変化）

Co-Authored-By: Claude Sonnet 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/bom/cyberdeck_bom.xlsx
+++ b/bom/cyberdeck_bom.xlsx
@@ -1377,7 +1377,7 @@
       </c>
       <c r="G21" s="15" t="inlineStr">
         <is>
-          <t>カーソル操作用 / FPC 6ピン 0.5mmピッチ 0.3mm厚 / 別途購入（AliExpress or 中古）</t>
+          <t>カーソル操作用 / FPC 4ピン 1.0mmピッチ / VCC=3.3V直結OK / ピンアサイン: GND-X-VCC-Y / 別途購入（AliExpress or 中古）</t>
         </is>
       </c>
     </row>
@@ -1394,17 +1394,17 @@
       </c>
       <c r="C22" s="14" t="inlineStr">
         <is>
-          <t>AFC01-S06FCA-00</t>
+          <t>Molex 5034800440</t>
         </is>
       </c>
       <c r="D22" s="14" t="inlineStr">
         <is>
-          <t>AFC01-S06FCA-00</t>
+          <t>5034800440</t>
         </is>
       </c>
       <c r="E22" s="14" t="inlineStr">
         <is>
-          <t>C262655</t>
+          <t>C3170007</t>
         </is>
       </c>
       <c r="F22" s="14" t="inlineStr">
@@ -1414,7 +1414,7 @@
       </c>
       <c r="G22" s="15" t="inlineStr">
         <is>
-          <t>6P 0.5mmピッチ Bottom Contact ZIF / 3DSスライドパッド接続用 / JLCPCB在庫52426個確認済み</t>
+          <t>4P 1.0mmピッチ ZIF ヒンジ式 両面接触 / 3DSスライドパッド接続用 / JLCPCB在庫928個</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix key count: 66 -> 63, fix keyboard-layout.json
- KLEを正確にパースして確認: 63キーが正しい数
- SKRPABE010: 68個→63個
- 1N4148W: 66個→63個
- keyboard-layout.json: 壊れていた外側[]を修正
- matrix.md: 合計キー数を63に修正
- BOM/Claude.md/PROJECT_PLAN.md全て更新

Co-Authored-By: Claude Sonnet 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/bom/cyberdeck_bom.xlsx
+++ b/bom/cyberdeck_bom.xlsx
@@ -1298,12 +1298,12 @@
       </c>
       <c r="F19" s="12" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>63</t>
         </is>
       </c>
       <c r="G19" s="13" t="inlineStr">
         <is>
-          <t>66キー + ショルダー2個 / 4.2×3.2mm SMD / JLCPCB在庫54355個確認済み</t>
+          <t>63キー / 4.2×3.2mm SMD / JLCPCB在庫54355個確認済み</t>
         </is>
       </c>
     </row>
@@ -1335,12 +1335,12 @@
       </c>
       <c r="F20" s="12" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>63</t>
         </is>
       </c>
       <c r="G20" s="13" t="inlineStr">
         <is>
-          <t>キーマトリクス用（66キー分）</t>
+          <t>キーマトリクス用（63キー分）</t>
         </is>
       </c>
     </row>

</xml_diff>